<commit_message>
Massive updates to the board
</commit_message>
<xml_diff>
--- a/ww101-shield/pin-bom.xlsx
+++ b/ww101-shield/pin-bom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="30720" yWindow="340" windowWidth="27720" windowHeight="26800" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="34800" yWindow="0" windowWidth="29300" windowHeight="27760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="pin-assignment" sheetId="1" r:id="rId1"/>
@@ -391,9 +391,6 @@
     <t>Therm-Ref-Hi</t>
   </si>
   <si>
-    <t>Therm-Low</t>
-  </si>
-  <si>
     <t>Therm-ref</t>
   </si>
   <si>
@@ -782,6 +779,9 @@
   </si>
   <si>
     <t>https://www.amazon.com/Diymall-Serial-128x64-Display-Arduino/dp/B01HHOETIA/ref=sr_1_15?ie=UTF8&amp;qid=1486828625&amp;sr=8-15&amp;keywords=0.96+I2C</t>
+  </si>
+  <si>
+    <t>Therm-low</t>
   </si>
 </sst>
 </file>
@@ -852,7 +852,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="104">
+  <cellStyleXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -951,6 +951,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -966,7 +968,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="97"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="104">
+  <cellStyles count="106">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1021,6 +1023,8 @@
     <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1406,9 +1410,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" zoomScalePageLayoutView="205" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" zoomScalePageLayoutView="205" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1420,7 +1424,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1429,7 +1433,7 @@
         <v>98</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>102</v>
@@ -1461,7 +1465,7 @@
         <v>118</v>
       </c>
       <c r="D2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E2" t="s">
         <v>54</v>
@@ -1478,7 +1482,7 @@
         <v>118</v>
       </c>
       <c r="D3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E3" t="s">
         <v>55</v>
@@ -1495,7 +1499,7 @@
         <v>119</v>
       </c>
       <c r="D4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E4" t="s">
         <v>56</v>
@@ -1535,7 +1539,7 @@
         <v>119</v>
       </c>
       <c r="D6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E6" t="s">
         <v>58</v>
@@ -1621,7 +1625,7 @@
         <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E10" t="s">
         <v>46</v>
@@ -1644,7 +1648,7 @@
         <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E11" t="s">
         <v>47</v>
@@ -1664,10 +1668,10 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E12" t="s">
         <v>48</v>
@@ -1675,10 +1679,10 @@
     </row>
     <row r="13" spans="1:12">
       <c r="C13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E13" t="s">
         <v>49</v>
@@ -1689,10 +1693,10 @@
     </row>
     <row r="14" spans="1:12">
       <c r="C14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E14" t="s">
         <v>50</v>
@@ -1703,10 +1707,10 @@
     </row>
     <row r="15" spans="1:12">
       <c r="C15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E15" t="s">
         <v>51</v>
@@ -1714,10 +1718,10 @@
     </row>
     <row r="16" spans="1:12">
       <c r="C16" t="s">
+        <v>156</v>
+      </c>
+      <c r="D16" t="s">
         <v>157</v>
-      </c>
-      <c r="D16" t="s">
-        <v>158</v>
       </c>
       <c r="E16" t="s">
         <v>52</v>
@@ -1725,10 +1729,10 @@
     </row>
     <row r="17" spans="1:9">
       <c r="C17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E17" t="s">
         <v>53</v>
@@ -1736,10 +1740,10 @@
     </row>
     <row r="18" spans="1:9">
       <c r="C18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E18" t="s">
         <v>38</v>
@@ -1747,10 +1751,10 @@
     </row>
     <row r="19" spans="1:9">
       <c r="C19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E19" t="s">
         <v>39</v>
@@ -1764,10 +1768,10 @@
     </row>
     <row r="20" spans="1:9">
       <c r="C20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E20" t="s">
         <v>40</v>
@@ -1778,7 +1782,7 @@
         <v>112</v>
       </c>
       <c r="D21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E21" t="s">
         <v>41</v>
@@ -1786,10 +1790,10 @@
     </row>
     <row r="22" spans="1:9">
       <c r="C22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E22" t="s">
         <v>42</v>
@@ -1797,10 +1801,10 @@
     </row>
     <row r="23" spans="1:9">
       <c r="C23" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E23" t="s">
         <v>43</v>
@@ -1808,10 +1812,10 @@
     </row>
     <row r="24" spans="1:9">
       <c r="C24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E24" t="s">
         <v>44</v>
@@ -1819,10 +1823,10 @@
     </row>
     <row r="25" spans="1:9">
       <c r="C25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E25" t="s">
         <v>45</v>
@@ -1833,7 +1837,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="C26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E26" t="s">
         <v>30</v>
@@ -1850,7 +1854,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="C27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E27" t="s">
         <v>31</v>
@@ -1867,7 +1871,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="C28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E28" t="s">
         <v>32</v>
@@ -1881,10 +1885,10 @@
     </row>
     <row r="29" spans="1:9">
       <c r="C29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E29" t="s">
         <v>33</v>
@@ -1921,7 +1925,7 @@
         <v>120</v>
       </c>
       <c r="D31" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E31" t="s">
         <v>35</v>
@@ -1932,10 +1936,10 @@
     </row>
     <row r="32" spans="1:9">
       <c r="C32" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D32" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="E32" t="s">
         <v>36</v>
@@ -1952,10 +1956,10 @@
     </row>
     <row r="33" spans="1:12">
       <c r="C33" t="s">
-        <v>121</v>
+        <v>252</v>
       </c>
       <c r="D33" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="E33" t="s">
         <v>37</v>
@@ -2018,10 +2022,10 @@
     </row>
     <row r="36" spans="1:12">
       <c r="C36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D36" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E36" t="s">
         <v>64</v>
@@ -2032,10 +2036,10 @@
     </row>
     <row r="37" spans="1:12">
       <c r="C37" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D37" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E37" t="s">
         <v>65</v>
@@ -2052,7 +2056,7 @@
         <v>100</v>
       </c>
       <c r="D38" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E38" t="s">
         <v>66</v>
@@ -2060,10 +2064,10 @@
     </row>
     <row r="39" spans="1:12">
       <c r="C39" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D39" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E39" t="s">
         <v>67</v>
@@ -2209,7 +2213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
@@ -2222,13 +2226,13 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C1" t="s">
         <v>115</v>
       </c>
       <c r="D1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E1" t="s">
         <v>106</v>
@@ -2242,10 +2246,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2253,10 +2257,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2264,7 +2268,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2272,7 +2276,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2280,10 +2284,10 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2291,13 +2295,13 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D7" t="s">
         <v>172</v>
-      </c>
-      <c r="D7" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2305,13 +2309,13 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D8" t="s">
         <v>172</v>
-      </c>
-      <c r="D8" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2319,13 +2323,13 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C9" t="s">
         <v>99</v>
       </c>
       <c r="D9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2333,13 +2337,13 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C10" t="s">
         <v>99</v>
       </c>
       <c r="D10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2347,13 +2351,13 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C11" t="s">
         <v>99</v>
       </c>
       <c r="D11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2361,13 +2365,13 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C12" t="s">
         <v>99</v>
       </c>
       <c r="D12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2375,13 +2379,13 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2389,13 +2393,13 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2403,13 +2407,13 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2417,13 +2421,13 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2431,19 +2435,19 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C17" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D17" t="s">
+        <v>198</v>
+      </c>
+      <c r="E17" t="s">
         <v>199</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" s="4" t="s">
         <v>200</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2451,19 +2455,19 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D18" t="s">
+        <v>198</v>
+      </c>
+      <c r="E18" t="s">
         <v>199</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>200</v>
-      </c>
-      <c r="F18" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2471,19 +2475,19 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D19" t="s">
+        <v>198</v>
+      </c>
+      <c r="E19" t="s">
         <v>199</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" s="4" t="s">
         <v>200</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2491,19 +2495,19 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
+        <v>197</v>
+      </c>
+      <c r="C20" t="s">
+        <v>189</v>
+      </c>
+      <c r="D20" t="s">
         <v>198</v>
       </c>
-      <c r="C20" t="s">
-        <v>190</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>199</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>200</v>
-      </c>
-      <c r="F20" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2511,16 +2515,16 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
+        <v>179</v>
+      </c>
+      <c r="C21" t="s">
         <v>180</v>
       </c>
-      <c r="C21" t="s">
-        <v>181</v>
-      </c>
       <c r="D21" t="s">
+        <v>204</v>
+      </c>
+      <c r="E21" t="s">
         <v>205</v>
-      </c>
-      <c r="E21" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2528,16 +2532,16 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -2545,16 +2549,16 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
+        <v>182</v>
+      </c>
+      <c r="C23" t="s">
         <v>183</v>
       </c>
-      <c r="C23" t="s">
-        <v>184</v>
-      </c>
       <c r="D23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -2562,19 +2566,19 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D24" t="s">
+        <v>198</v>
+      </c>
+      <c r="E24" t="s">
         <v>199</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" s="4" t="s">
         <v>200</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -2582,19 +2586,19 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D25" t="s">
+        <v>198</v>
+      </c>
+      <c r="E25" t="s">
         <v>199</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>200</v>
-      </c>
-      <c r="F25" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -2602,13 +2606,13 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C26" t="s">
+        <v>183</v>
+      </c>
+      <c r="D26" t="s">
         <v>184</v>
-      </c>
-      <c r="D26" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -2616,13 +2620,13 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C27" t="s">
+        <v>183</v>
+      </c>
+      <c r="D27" t="s">
         <v>184</v>
-      </c>
-      <c r="D27" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -2630,19 +2634,19 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D28" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E28" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F28" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -2650,19 +2654,19 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C29" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -2670,13 +2674,13 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C30" t="s">
+        <v>249</v>
+      </c>
+      <c r="D30" t="s">
         <v>250</v>
-      </c>
-      <c r="D30" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -2684,13 +2688,13 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C31" t="s">
+        <v>249</v>
+      </c>
+      <c r="D31" t="s">
         <v>250</v>
-      </c>
-      <c r="D31" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -2698,13 +2702,13 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C32" t="s">
+        <v>249</v>
+      </c>
+      <c r="D32" t="s">
         <v>250</v>
-      </c>
-      <c r="D32" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -2712,13 +2716,13 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
+        <v>248</v>
+      </c>
+      <c r="C33" t="s">
         <v>249</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>250</v>
-      </c>
-      <c r="D33" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -2746,16 +2750,16 @@
         <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C36" t="s">
         <v>29</v>
       </c>
       <c r="D36" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E36" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -2763,19 +2767,19 @@
         <v>4</v>
       </c>
       <c r="B37" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C37" t="s">
         <v>29</v>
       </c>
       <c r="D37" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F37" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -2783,7 +2787,7 @@
         <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C38" t="s">
         <v>104</v>
@@ -2803,16 +2807,16 @@
         <v>4</v>
       </c>
       <c r="B39" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C39" t="s">
         <v>104</v>
       </c>
       <c r="D39" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E39" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -2820,7 +2824,7 @@
         <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C40" t="s">
         <v>112</v>
@@ -2840,16 +2844,16 @@
         <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C41" t="s">
         <v>112</v>
       </c>
       <c r="D41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E41" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -2857,16 +2861,16 @@
         <v>2</v>
       </c>
       <c r="B43" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C43" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D43" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -2874,16 +2878,16 @@
         <v>2</v>
       </c>
       <c r="B44" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C44" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D44" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -2891,16 +2895,16 @@
         <v>2</v>
       </c>
       <c r="B45" t="s">
+        <v>219</v>
+      </c>
+      <c r="C45" t="s">
         <v>220</v>
       </c>
-      <c r="C45" t="s">
-        <v>221</v>
-      </c>
       <c r="D45" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E45" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -2908,16 +2912,16 @@
         <v>2</v>
       </c>
       <c r="B46" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C46" t="s">
         <v>19</v>
       </c>
       <c r="D46" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -2925,16 +2929,16 @@
         <v>2</v>
       </c>
       <c r="B47" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C47" t="s">
         <v>19</v>
       </c>
       <c r="D47" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E47" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -2942,16 +2946,16 @@
         <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C48" t="s">
         <v>19</v>
       </c>
       <c r="D48" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E48" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -2959,16 +2963,16 @@
         <v>2</v>
       </c>
       <c r="B49" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C49" t="s">
         <v>19</v>
       </c>
       <c r="D49" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E49" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -2976,16 +2980,16 @@
         <v>2</v>
       </c>
       <c r="B50" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C50" t="s">
         <v>19</v>
       </c>
       <c r="D50" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -2993,16 +2997,16 @@
         <v>2</v>
       </c>
       <c r="B51" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C51" t="s">
         <v>19</v>
       </c>
       <c r="D51" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E51" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -3010,16 +3014,16 @@
         <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C52" t="s">
         <v>19</v>
       </c>
       <c r="D52" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E52" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -3027,16 +3031,16 @@
         <v>2</v>
       </c>
       <c r="B53" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C53" t="s">
         <v>19</v>
       </c>
       <c r="D53" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E53" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -3044,16 +3048,16 @@
         <v>2</v>
       </c>
       <c r="B54" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C54" t="s">
         <v>19</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E54" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -3061,13 +3065,13 @@
         <v>2</v>
       </c>
       <c r="B55" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C55" t="s">
+        <v>127</v>
+      </c>
+      <c r="D55" t="s">
         <v>128</v>
-      </c>
-      <c r="D55" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -3075,13 +3079,13 @@
         <v>3</v>
       </c>
       <c r="B58" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C58" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D58" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -3089,13 +3093,13 @@
         <v>3</v>
       </c>
       <c r="B59" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C59" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D59" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Consolidated all BOM/Pinout Spreadsheets
</commit_message>
<xml_diff>
--- a/ww101-shield/pin-bom.xlsx
+++ b/ww101-shield/pin-bom.xlsx
@@ -9,14 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="27100" yWindow="1020" windowWidth="28800" windowHeight="26000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="pin-assignment" sheetId="1" r:id="rId1"/>
-    <sheet name="BOM" sheetId="2" r:id="rId2"/>
+    <sheet name="BASEMAPV22" sheetId="5" r:id="rId1"/>
+    <sheet name="PINV22" sheetId="4" r:id="rId2"/>
+    <sheet name="V22 BOM" sheetId="3" r:id="rId3"/>
+    <sheet name="PINV1X" sheetId="1" r:id="rId4"/>
+    <sheet name="BOMV1X" sheetId="2" r:id="rId5"/>
+    <sheet name="BASEMAPV1x" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'pin-assignment'!$A$1:$E$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">PINV1X!$A$1:$E$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PINV22!$A$1:$D$51</definedName>
+    <definedName name="ww101board" localSheetId="2">'V22 BOM'!$A$1:$E$63</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -30,8 +36,27 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="ww101board" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/arh/Documents/iotexpert-projects/WA101/ww101-shield/eagle/ww101board.csv" tab="0" semicolon="1">
+      <textFields count="8">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="379">
   <si>
     <t>Arduino</t>
   </si>
@@ -724,13 +749,476 @@
   </si>
   <si>
     <t>MB2/swdata</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Device</t>
+  </si>
+  <si>
+    <t>Package</t>
+  </si>
+  <si>
+    <t>1uF</t>
+  </si>
+  <si>
+    <t>CAP0603-CAP</t>
+  </si>
+  <si>
+    <t>0603-CAP</t>
+  </si>
+  <si>
+    <t>Capacitor</t>
+  </si>
+  <si>
+    <t>0.1uF</t>
+  </si>
+  <si>
+    <t>180pF</t>
+  </si>
+  <si>
+    <t>2.2nF</t>
+  </si>
+  <si>
+    <t>10nF</t>
+  </si>
+  <si>
+    <t>C15</t>
+  </si>
+  <si>
+    <t>C16</t>
+  </si>
+  <si>
+    <t>C17</t>
+  </si>
+  <si>
+    <t>10uF</t>
+  </si>
+  <si>
+    <t>CLED0</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>LEDCHIP-LED0603</t>
+  </si>
+  <si>
+    <t>CHIP-LED0603</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>CLED1</t>
+  </si>
+  <si>
+    <t>CLED2</t>
+  </si>
+  <si>
+    <t>CLED3</t>
+  </si>
+  <si>
+    <t>Ambient Light Sensor Vishay TEMD6200FX01 http://www.vishay.com/docs/81812/temd6200.pdf</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>DNP</t>
+  </si>
+  <si>
+    <t>JMP-3-PTH-PTH</t>
+  </si>
+  <si>
+    <t>JMP-3-NO-PTH-2.54</t>
+  </si>
+  <si>
+    <t>Three Terminal Jumper - Normally Open</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>U8G-096-OLED</t>
+  </si>
+  <si>
+    <t>096-SSD1306</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>M05LOCK</t>
+  </si>
+  <si>
+    <t>1X05_LOCK</t>
+  </si>
+  <si>
+    <t>Header 5</t>
+  </si>
+  <si>
+    <t>SWITCH</t>
+  </si>
+  <si>
+    <t>PROX</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>RESISTOR0603</t>
+  </si>
+  <si>
+    <t>0603-RES</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>TRIM_US-3386P</t>
+  </si>
+  <si>
+    <t>3386P</t>
+  </si>
+  <si>
+    <t>POTENTIOMETER</t>
+  </si>
+  <si>
+    <t>10K Thermister</t>
+  </si>
+  <si>
+    <t>THERMISTOR-5</t>
+  </si>
+  <si>
+    <t>R-5</t>
+  </si>
+  <si>
+    <t>THERMISTOR</t>
+  </si>
+  <si>
+    <t>220K</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>0R</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>R26</t>
+  </si>
+  <si>
+    <t>R27</t>
+  </si>
+  <si>
+    <t>50K</t>
+  </si>
+  <si>
+    <t>JMP-3-1_2</t>
+  </si>
+  <si>
+    <t>Three Terminal Jumper - 1 &amp; 2 Connected</t>
+  </si>
+  <si>
+    <t>JMP-3-2_3</t>
+  </si>
+  <si>
+    <t>Three Terminal Jumper - 2 &amp; 3 Connected</t>
+  </si>
+  <si>
+    <t>R32</t>
+  </si>
+  <si>
+    <t>JMP-3-NO</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>CY8C4A45-48</t>
+  </si>
+  <si>
+    <t>TQFP-7X7-48</t>
+  </si>
+  <si>
+    <t>Arduino
+Pin</t>
+  </si>
+  <si>
+    <t>AFE Shield</t>
+  </si>
+  <si>
+    <t>CYW943907AEVAL1F</t>
+  </si>
+  <si>
+    <t>CYW920706WCDEVAL</t>
+  </si>
+  <si>
+    <t>Pin</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>External ADC</t>
+  </si>
+  <si>
+    <t>BT_GPIO_5/P15</t>
+  </si>
+  <si>
+    <t>Also debug pin and VBAT jumpers</t>
+  </si>
+  <si>
+    <t>DAC</t>
+  </si>
+  <si>
+    <t>I2C</t>
+  </si>
+  <si>
+    <t>External ADC or I2C (res change)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2S_PCM_OUT/P3/P29/P35 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2S_PCM_IN/P12 </t>
+  </si>
+  <si>
+    <t>Rx</t>
+  </si>
+  <si>
+    <t>WICED_GPIO_1</t>
+  </si>
+  <si>
+    <t>BT_UART_RXD</t>
+  </si>
+  <si>
+    <t>Tx</t>
+  </si>
+  <si>
+    <t>WICED_GPIO_2</t>
+  </si>
+  <si>
+    <t>BT_UART_TXD</t>
+  </si>
+  <si>
+    <t>WICED_GPIO_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2S_WS_PCM_SYNC/P0/P345 </t>
+  </si>
+  <si>
+    <t>PUART 2nd Option</t>
+  </si>
+  <si>
+    <t>WICED_GPIO_3</t>
+  </si>
+  <si>
+    <t>WICED_PWM_6</t>
+  </si>
+  <si>
+    <t>WICED_GPIO_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BT_GPIO_7/P30 </t>
+  </si>
+  <si>
+    <t>Baseboard button</t>
+  </si>
+  <si>
+    <t>WICED_GPIO_12</t>
+  </si>
+  <si>
+    <t>WICED_PWM_3</t>
+  </si>
+  <si>
+    <t>BT_GPIO_6/P11/P26</t>
+  </si>
+  <si>
+    <t>PWM0 and Baseboard LED</t>
+  </si>
+  <si>
+    <t>WICED_GPIO_11</t>
+  </si>
+  <si>
+    <t>WICED_PWM_4 and LED1</t>
+  </si>
+  <si>
+    <t>WICED_GPIO_31</t>
+  </si>
+  <si>
+    <t>WICED_GPIO_36</t>
+  </si>
+  <si>
+    <t>WICED_GPIO_17</t>
+  </si>
+  <si>
+    <t>WICED_PWM_5</t>
+  </si>
+  <si>
+    <t>WICED_GPIO_7</t>
+  </si>
+  <si>
+    <t>WICED_PWM_2</t>
+  </si>
+  <si>
+    <t>BT_DEV_WAKE/P36/P38</t>
+  </si>
+  <si>
+    <t>WICED_GPIO_6</t>
+  </si>
+  <si>
+    <t>WICED_PWM_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BT_GPIO_3/P27/P33 </t>
+  </si>
+  <si>
+    <t>PWM1</t>
+  </si>
+  <si>
+    <t>WICED_GPIO_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BT_HOST_WAKE/P25/P32 </t>
+  </si>
+  <si>
+    <t>CapSense Int</t>
+  </si>
+  <si>
+    <t>WICED_GPIO_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BT_CLK_REQ/P4/P24 </t>
+  </si>
+  <si>
+    <t>D18</t>
+  </si>
+  <si>
+    <t>WICED_GPIO_48</t>
+  </si>
+  <si>
+    <t>WICED_I2C_2 or WICED_I2C_1 (res change)</t>
+  </si>
+  <si>
+    <t>D19</t>
+  </si>
+  <si>
+    <t>WICED_GPIO_49</t>
+  </si>
+  <si>
+    <t>CYW92070xV3_EVAL</t>
+  </si>
+  <si>
+    <t>CYW9207X9WCDEVAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BT_DEV_WAKE/P36/P38 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2S_PCM_CLK/P2/P28/P37 </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PUART 2nd Option</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and RST_ARD?</t>
+    </r>
+  </si>
+  <si>
+    <t>Debug Pin?</t>
+  </si>
+  <si>
+    <t>LED0</t>
+  </si>
+  <si>
+    <t>I2C Control</t>
+  </si>
+  <si>
+    <t>D14</t>
+  </si>
+  <si>
+    <t>D15</t>
+  </si>
+  <si>
+    <t>ALS  (from 0 Ohm)</t>
+  </si>
+  <si>
+    <t>FUTUREARD</t>
+  </si>
+  <si>
+    <t>Capsense Int</t>
+  </si>
+  <si>
+    <t>ARD-MB1</t>
+  </si>
+  <si>
+    <t>ARD-LED1</t>
+  </si>
+  <si>
+    <t>ARD-LED2</t>
+  </si>
+  <si>
+    <t>ARD-MB2</t>
+  </si>
+  <si>
+    <t>Future Ardino</t>
+  </si>
+  <si>
+    <t>ALS (through 0 ohm resistor)</t>
+  </si>
+  <si>
+    <t>MB1/swdata</t>
+  </si>
+  <si>
+    <t>MB2/swclock</t>
+  </si>
+  <si>
+    <t>CAP-PSOC</t>
+  </si>
+  <si>
+    <t>PROXLED</t>
+  </si>
+  <si>
+    <t>GND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -768,8 +1256,36 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -788,8 +1304,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -797,8 +1319,116 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="106">
+  <cellStyleXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -905,8 +1535,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -916,8 +1547,56 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="106" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="106" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="106" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="106" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="106" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="106"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="106" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="106" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="106" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="106" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="106" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="106" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="106" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="106" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="106" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="106" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="106" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="106" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="106" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="106" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="106" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="106" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="106" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="106" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="106" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="106" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="106">
+  <cellStyles count="107">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1024,6 +1703,7 @@
     <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="97" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="106"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1033,6 +1713,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ww101board" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1357,10 +2041,2170 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScale="126" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5" style="16" customWidth="1"/>
+    <col min="4" max="4" width="19" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.1640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.5" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="E1" s="15"/>
+      <c r="F1" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="G1" s="15"/>
+    </row>
+    <row r="2" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>303</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>303</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="B3" s="21"/>
+      <c r="C3" s="22" t="s">
+        <v>373</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>305</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>306</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>307</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="22" t="s">
+        <v>309</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>305</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>306</v>
+      </c>
+      <c r="F4" s="20"/>
+      <c r="G4" s="25"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="21"/>
+      <c r="C5" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>305</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>306</v>
+      </c>
+      <c r="F5" s="20"/>
+      <c r="G5" s="21"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="20" t="s">
+        <v>305</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>306</v>
+      </c>
+      <c r="F6" s="20"/>
+      <c r="G6" s="21"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>310</v>
+      </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="20" t="s">
+        <v>305</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>311</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>312</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>310</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="20" t="s">
+        <v>305</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>311</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>314</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>314</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>315</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>314</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>316</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>317</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>317</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>318</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>317</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>319</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="21"/>
+      <c r="C11" s="16" t="s">
+        <v>372</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>320</v>
+      </c>
+      <c r="E11" s="21"/>
+      <c r="F11" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>323</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>324</v>
+      </c>
+      <c r="F12" s="20"/>
+      <c r="G12" s="21"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="21"/>
+      <c r="C13" s="27" t="s">
+        <v>368</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>325</v>
+      </c>
+      <c r="E13" s="21"/>
+      <c r="F13" s="20" t="s">
+        <v>326</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>369</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>328</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>329</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>330</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>332</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>333</v>
+      </c>
+      <c r="F15" s="20"/>
+      <c r="G15" s="21"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="21"/>
+      <c r="D16" s="20" t="s">
+        <v>334</v>
+      </c>
+      <c r="E16" s="21"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="21"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="21"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="E17" s="21"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="21"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="22"/>
+      <c r="D18" s="20" t="s">
+        <v>336</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>337</v>
+      </c>
+      <c r="F18" s="20"/>
+      <c r="G18" s="21"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="22"/>
+      <c r="D19" s="20" t="s">
+        <v>338</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>339</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>340</v>
+      </c>
+      <c r="G19" s="21"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>370</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>342</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="G20" s="21" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="21"/>
+      <c r="C21" s="29" t="s">
+        <v>371</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>345</v>
+      </c>
+      <c r="E21" s="21"/>
+      <c r="F21" s="20" t="s">
+        <v>346</v>
+      </c>
+      <c r="G21" s="21"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="21"/>
+      <c r="C22" s="29" t="s">
+        <v>347</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>348</v>
+      </c>
+      <c r="E22" s="21"/>
+      <c r="F22" s="20" t="s">
+        <v>349</v>
+      </c>
+      <c r="G22" s="21"/>
+    </row>
+    <row r="23" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="26" t="s">
+        <v>350</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>310</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>310</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>351</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>352</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>312</v>
+      </c>
+      <c r="G23" s="21" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="30" t="s">
+        <v>353</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>310</v>
+      </c>
+      <c r="C24" s="32" t="s">
+        <v>310</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>354</v>
+      </c>
+      <c r="E24" s="31" t="s">
+        <v>352</v>
+      </c>
+      <c r="F24" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="G24" s="31" t="s">
+        <v>310</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" zoomScalePageLayoutView="205" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="4"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B2" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>222</v>
+      </c>
+      <c r="C3" t="s">
+        <v>375</v>
+      </c>
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>371</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C6" t="s">
+        <v>223</v>
+      </c>
+      <c r="D6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>224</v>
+      </c>
+      <c r="C8" t="s">
+        <v>224</v>
+      </c>
+      <c r="D8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16" t="s">
+        <v>124</v>
+      </c>
+      <c r="D16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" t="s">
+        <v>126</v>
+      </c>
+      <c r="D18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" t="s">
+        <v>129</v>
+      </c>
+      <c r="D20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" t="s">
+        <v>131</v>
+      </c>
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>134</v>
+      </c>
+      <c r="C22" t="s">
+        <v>132</v>
+      </c>
+      <c r="D22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>133</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="D23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" t="s">
+        <v>127</v>
+      </c>
+      <c r="D24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>219</v>
+      </c>
+      <c r="C26" t="s">
+        <v>377</v>
+      </c>
+      <c r="D26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>133</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" t="s">
+        <v>122</v>
+      </c>
+      <c r="D32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>218</v>
+      </c>
+      <c r="C33" t="s">
+        <v>378</v>
+      </c>
+      <c r="D33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>114</v>
+      </c>
+      <c r="C36" t="s">
+        <v>118</v>
+      </c>
+      <c r="D36" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>115</v>
+      </c>
+      <c r="C37" t="s">
+        <v>119</v>
+      </c>
+      <c r="D37" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>136</v>
+      </c>
+      <c r="C39" t="s">
+        <v>136</v>
+      </c>
+      <c r="D39" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D51">
+    <sortState ref="A2:D51">
+      <sortCondition ref="D1:D51"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E63"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" style="9" customWidth="1"/>
+    <col min="3" max="3" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="C1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D1" t="s">
+        <v>233</v>
+      </c>
+      <c r="E1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="C3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D3" t="s">
+        <v>236</v>
+      </c>
+      <c r="E3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C4" t="s">
+        <v>235</v>
+      </c>
+      <c r="D4" t="s">
+        <v>236</v>
+      </c>
+      <c r="E4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="C5" t="s">
+        <v>235</v>
+      </c>
+      <c r="D5" t="s">
+        <v>236</v>
+      </c>
+      <c r="E5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C6" t="s">
+        <v>235</v>
+      </c>
+      <c r="D6" t="s">
+        <v>236</v>
+      </c>
+      <c r="E6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="C7" t="s">
+        <v>235</v>
+      </c>
+      <c r="D7" t="s">
+        <v>236</v>
+      </c>
+      <c r="E7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="C8" t="s">
+        <v>235</v>
+      </c>
+      <c r="D8" t="s">
+        <v>236</v>
+      </c>
+      <c r="E8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D9" t="s">
+        <v>236</v>
+      </c>
+      <c r="E9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="C10" t="s">
+        <v>235</v>
+      </c>
+      <c r="D10" t="s">
+        <v>236</v>
+      </c>
+      <c r="E10" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>210</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="C11" t="s">
+        <v>235</v>
+      </c>
+      <c r="D11" t="s">
+        <v>236</v>
+      </c>
+      <c r="E11" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>204</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="C12" t="s">
+        <v>235</v>
+      </c>
+      <c r="D12" t="s">
+        <v>236</v>
+      </c>
+      <c r="E12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>183</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="C13" t="s">
+        <v>235</v>
+      </c>
+      <c r="D13" t="s">
+        <v>236</v>
+      </c>
+      <c r="E13" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>184</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C14" t="s">
+        <v>235</v>
+      </c>
+      <c r="D14" t="s">
+        <v>236</v>
+      </c>
+      <c r="E14" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>185</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="C15" t="s">
+        <v>235</v>
+      </c>
+      <c r="D15" t="s">
+        <v>236</v>
+      </c>
+      <c r="E15" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>242</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="C16" t="s">
+        <v>235</v>
+      </c>
+      <c r="D16" t="s">
+        <v>236</v>
+      </c>
+      <c r="E16" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>243</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="C17" t="s">
+        <v>235</v>
+      </c>
+      <c r="D17" t="s">
+        <v>236</v>
+      </c>
+      <c r="E17" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>244</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="C18" t="s">
+        <v>235</v>
+      </c>
+      <c r="D18" t="s">
+        <v>236</v>
+      </c>
+      <c r="E18" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>246</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="C19" t="s">
+        <v>248</v>
+      </c>
+      <c r="D19" t="s">
+        <v>249</v>
+      </c>
+      <c r="E19" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>251</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="C20" t="s">
+        <v>248</v>
+      </c>
+      <c r="D20" t="s">
+        <v>249</v>
+      </c>
+      <c r="E20" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>252</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="C21" t="s">
+        <v>248</v>
+      </c>
+      <c r="D21" t="s">
+        <v>249</v>
+      </c>
+      <c r="E21" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>253</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="C22" t="s">
+        <v>248</v>
+      </c>
+      <c r="D22" t="s">
+        <v>249</v>
+      </c>
+      <c r="E22" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>131</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>255</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="C25" t="s">
+        <v>257</v>
+      </c>
+      <c r="D25" t="s">
+        <v>258</v>
+      </c>
+      <c r="E25" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>260</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="C26" t="s">
+        <v>261</v>
+      </c>
+      <c r="D26" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>263</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="C27" t="s">
+        <v>264</v>
+      </c>
+      <c r="D27" t="s">
+        <v>265</v>
+      </c>
+      <c r="E27" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>224</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="C28" t="s">
+        <v>248</v>
+      </c>
+      <c r="D28" t="s">
+        <v>249</v>
+      </c>
+      <c r="E28" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>223</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="C29" t="s">
+        <v>248</v>
+      </c>
+      <c r="D29" t="s">
+        <v>249</v>
+      </c>
+      <c r="E29" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>107</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="C30" t="s">
+        <v>168</v>
+      </c>
+      <c r="D30" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>222</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="C31" t="s">
+        <v>168</v>
+      </c>
+      <c r="D31" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>268</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="C32" t="s">
+        <v>248</v>
+      </c>
+      <c r="D32" t="s">
+        <v>249</v>
+      </c>
+      <c r="E32" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>199</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="C33" t="s">
+        <v>270</v>
+      </c>
+      <c r="D33" t="s">
+        <v>271</v>
+      </c>
+      <c r="E33" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>145</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="C34" t="s">
+        <v>273</v>
+      </c>
+      <c r="D34" t="s">
+        <v>274</v>
+      </c>
+      <c r="E34" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>156</v>
+      </c>
+      <c r="B35" s="9">
+        <v>560</v>
+      </c>
+      <c r="C35" t="s">
+        <v>270</v>
+      </c>
+      <c r="D35" t="s">
+        <v>271</v>
+      </c>
+      <c r="E35" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>157</v>
+      </c>
+      <c r="B36" s="9">
+        <v>560</v>
+      </c>
+      <c r="C36" t="s">
+        <v>270</v>
+      </c>
+      <c r="D36" t="s">
+        <v>271</v>
+      </c>
+      <c r="E36" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>158</v>
+      </c>
+      <c r="B37" s="9">
+        <v>560</v>
+      </c>
+      <c r="C37" t="s">
+        <v>270</v>
+      </c>
+      <c r="D37" t="s">
+        <v>271</v>
+      </c>
+      <c r="E37" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>159</v>
+      </c>
+      <c r="B38" s="9">
+        <v>560</v>
+      </c>
+      <c r="C38" t="s">
+        <v>270</v>
+      </c>
+      <c r="D38" t="s">
+        <v>271</v>
+      </c>
+      <c r="E38" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>147</v>
+      </c>
+      <c r="B39" s="9">
+        <v>560</v>
+      </c>
+      <c r="C39" t="s">
+        <v>270</v>
+      </c>
+      <c r="D39" t="s">
+        <v>271</v>
+      </c>
+      <c r="E39" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>148</v>
+      </c>
+      <c r="B40" s="9">
+        <v>560</v>
+      </c>
+      <c r="C40" t="s">
+        <v>270</v>
+      </c>
+      <c r="D40" t="s">
+        <v>271</v>
+      </c>
+      <c r="E40" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>151</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="C41" t="s">
+        <v>270</v>
+      </c>
+      <c r="D41" t="s">
+        <v>271</v>
+      </c>
+      <c r="E41" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>152</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="C42" t="s">
+        <v>270</v>
+      </c>
+      <c r="D42" t="s">
+        <v>271</v>
+      </c>
+      <c r="E42" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>200</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="C43" t="s">
+        <v>277</v>
+      </c>
+      <c r="D43" t="s">
+        <v>278</v>
+      </c>
+      <c r="E43" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>209</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="C44" t="s">
+        <v>270</v>
+      </c>
+      <c r="D44" t="s">
+        <v>271</v>
+      </c>
+      <c r="E44" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>141</v>
+      </c>
+      <c r="B45" s="9">
+        <v>560</v>
+      </c>
+      <c r="C45" t="s">
+        <v>270</v>
+      </c>
+      <c r="D45" t="s">
+        <v>271</v>
+      </c>
+      <c r="E45" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>142</v>
+      </c>
+      <c r="B46" s="9">
+        <v>560</v>
+      </c>
+      <c r="C46" t="s">
+        <v>270</v>
+      </c>
+      <c r="D46" t="s">
+        <v>271</v>
+      </c>
+      <c r="E46" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>143</v>
+      </c>
+      <c r="B47" s="9">
+        <v>560</v>
+      </c>
+      <c r="C47" t="s">
+        <v>270</v>
+      </c>
+      <c r="D47" t="s">
+        <v>271</v>
+      </c>
+      <c r="E47" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>144</v>
+      </c>
+      <c r="B48" s="9">
+        <v>560</v>
+      </c>
+      <c r="C48" t="s">
+        <v>270</v>
+      </c>
+      <c r="D48" t="s">
+        <v>271</v>
+      </c>
+      <c r="E48" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>281</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="C49" t="s">
+        <v>270</v>
+      </c>
+      <c r="D49" t="s">
+        <v>271</v>
+      </c>
+      <c r="E49" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>211</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="C50" t="s">
+        <v>270</v>
+      </c>
+      <c r="D50" t="s">
+        <v>271</v>
+      </c>
+      <c r="E50" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>212</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="C51" t="s">
+        <v>270</v>
+      </c>
+      <c r="D51" t="s">
+        <v>271</v>
+      </c>
+      <c r="E51" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>213</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="C52" t="s">
+        <v>270</v>
+      </c>
+      <c r="D52" t="s">
+        <v>271</v>
+      </c>
+      <c r="E52" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>214</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="C53" t="s">
+        <v>270</v>
+      </c>
+      <c r="D53" t="s">
+        <v>271</v>
+      </c>
+      <c r="E53" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>283</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="C54" t="s">
+        <v>270</v>
+      </c>
+      <c r="D54" t="s">
+        <v>271</v>
+      </c>
+      <c r="E54" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>284</v>
+      </c>
+      <c r="B55" s="9">
+        <v>560</v>
+      </c>
+      <c r="C55" t="s">
+        <v>270</v>
+      </c>
+      <c r="D55" t="s">
+        <v>271</v>
+      </c>
+      <c r="E55" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>285</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="C56" t="s">
+        <v>270</v>
+      </c>
+      <c r="D56" t="s">
+        <v>271</v>
+      </c>
+      <c r="E56" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>286</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="C57" t="s">
+        <v>270</v>
+      </c>
+      <c r="D57" t="s">
+        <v>271</v>
+      </c>
+      <c r="E57" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>287</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="C58" t="s">
+        <v>270</v>
+      </c>
+      <c r="D58" t="s">
+        <v>271</v>
+      </c>
+      <c r="E58" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>288</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="C59" t="s">
+        <v>270</v>
+      </c>
+      <c r="D59" t="s">
+        <v>271</v>
+      </c>
+      <c r="E59" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>153</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="C60" t="s">
+        <v>270</v>
+      </c>
+      <c r="D60" t="s">
+        <v>290</v>
+      </c>
+      <c r="E60" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>154</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="C61" t="s">
+        <v>270</v>
+      </c>
+      <c r="D61" t="s">
+        <v>292</v>
+      </c>
+      <c r="E61" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>294</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="C62" t="s">
+        <v>270</v>
+      </c>
+      <c r="D62" t="s">
+        <v>295</v>
+      </c>
+      <c r="E62" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>296</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="C63" t="s">
+        <v>297</v>
+      </c>
+      <c r="D63" t="s">
+        <v>298</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" zoomScalePageLayoutView="205" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" zoomScalePageLayoutView="205" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
@@ -1978,11 +4822,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
@@ -2880,4 +5724,553 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.1640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.83203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5" style="16" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" style="16" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="E1" s="15"/>
+      <c r="F1" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="G1" s="15"/>
+      <c r="H1" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="I1" s="15"/>
+    </row>
+    <row r="2" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>303</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>303</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>303</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="B3" s="21"/>
+      <c r="C3" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>305</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>306</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>357</v>
+      </c>
+      <c r="G3" s="21"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="21"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="22" t="s">
+        <v>309</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>305</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>306</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>358</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>359</v>
+      </c>
+      <c r="H4" s="20"/>
+      <c r="I4" s="21"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="21"/>
+      <c r="C5" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>305</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>306</v>
+      </c>
+      <c r="F5" s="34" t="s">
+        <v>307</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>360</v>
+      </c>
+      <c r="H5" s="20"/>
+      <c r="I5" s="21"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="20" t="s">
+        <v>305</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>306</v>
+      </c>
+      <c r="F6" s="34"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="21"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>310</v>
+      </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="20" t="s">
+        <v>305</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>311</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>312</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>310</v>
+      </c>
+      <c r="H7" s="20"/>
+      <c r="I7" s="21"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>310</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="20" t="s">
+        <v>305</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>311</v>
+      </c>
+      <c r="F8" s="34" t="s">
+        <v>313</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>310</v>
+      </c>
+      <c r="H8" s="20"/>
+      <c r="I8" s="21"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>314</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>314</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>315</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>314</v>
+      </c>
+      <c r="F9" s="34" t="s">
+        <v>316</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>314</v>
+      </c>
+      <c r="H9" s="20"/>
+      <c r="I9" s="21"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>317</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>317</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>318</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>317</v>
+      </c>
+      <c r="F10" s="34" t="s">
+        <v>319</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>317</v>
+      </c>
+      <c r="H10" s="20"/>
+      <c r="I10" s="21"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="21"/>
+      <c r="C11" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>320</v>
+      </c>
+      <c r="E11" s="21"/>
+      <c r="F11" s="34" t="s">
+        <v>321</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>322</v>
+      </c>
+      <c r="H11" s="20"/>
+      <c r="I11" s="21"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>361</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>323</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>324</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>343</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>344</v>
+      </c>
+      <c r="H12" s="20"/>
+      <c r="I12" s="21"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="21"/>
+      <c r="C13" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>325</v>
+      </c>
+      <c r="E13" s="21"/>
+      <c r="F13" s="34" t="s">
+        <v>326</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>327</v>
+      </c>
+      <c r="H13" s="20"/>
+      <c r="I13" s="21"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>224</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>328</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>329</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>330</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>331</v>
+      </c>
+      <c r="H14" s="20"/>
+      <c r="I14" s="21"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>332</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>333</v>
+      </c>
+      <c r="F15" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="G15" s="21"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="21"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="21"/>
+      <c r="C16" s="22" t="s">
+        <v>362</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>334</v>
+      </c>
+      <c r="E16" s="21"/>
+      <c r="F16" s="34" t="s">
+        <v>349</v>
+      </c>
+      <c r="G16" s="21"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="21"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="21"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="E17" s="21"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="21"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="22"/>
+      <c r="D18" s="20" t="s">
+        <v>336</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>337</v>
+      </c>
+      <c r="F18" s="34"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="21"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="22"/>
+      <c r="D19" s="20" t="s">
+        <v>338</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>339</v>
+      </c>
+      <c r="F19" s="34"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="21"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="22"/>
+      <c r="D20" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>342</v>
+      </c>
+      <c r="F20" s="34"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="21"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="21"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="20" t="s">
+        <v>345</v>
+      </c>
+      <c r="E21" s="21"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="21"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="21"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="20" t="s">
+        <v>348</v>
+      </c>
+      <c r="E22" s="21"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="21"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="20" t="s">
+        <v>363</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>310</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>310</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>351</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>352</v>
+      </c>
+      <c r="F23" s="34" t="s">
+        <v>312</v>
+      </c>
+      <c r="G23" s="21" t="s">
+        <v>310</v>
+      </c>
+      <c r="H23" s="20"/>
+      <c r="I23" s="21"/>
+    </row>
+    <row r="24" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="33" t="s">
+        <v>364</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>310</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>310</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>354</v>
+      </c>
+      <c r="E24" s="31" t="s">
+        <v>352</v>
+      </c>
+      <c r="F24" s="36" t="s">
+        <v>313</v>
+      </c>
+      <c r="G24" s="31" t="s">
+        <v>310</v>
+      </c>
+      <c r="H24" s="33"/>
+      <c r="I24" s="31"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>